<commit_message>
ajout commentaire test test_checkSkittlesInTen
</commit_message>
<xml_diff>
--- a/tests/test_cases_recipes.xlsx
+++ b/tests/test_cases_recipes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\canad\Documents\APP4\INFO\bowlingP\bowling_project\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF2A9755-20FA-40F6-AB6B-0DF6E34440A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A55B2E2-3710-4FF7-BC24-BAF68B88EC94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
   <si>
     <t>Test Name</t>
   </si>
@@ -47,9 +47,6 @@
     <t>Validation</t>
   </si>
   <si>
-    <t>__init__</t>
-  </si>
-  <si>
     <t>add_scores_to_frame</t>
   </si>
   <si>
@@ -144,13 +141,54 @@
   </si>
   <si>
     <t>error</t>
+  </si>
+  <si>
+    <r>
+      <t>Player(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6897BB"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFCC7832"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6A8759"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>"David"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -173,11 +211,22 @@
       <family val="3"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF00B050"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <sz val="10"/>
+      <color rgb="FFA9B7C6"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF6897BB"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF6A8759"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -223,7 +272,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -539,10 +590,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -570,7 +621,6 @@
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
@@ -581,19 +631,23 @@
       <c r="A4" t="s">
         <v>6</v>
       </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4" t="str">
+        <f>IF(C4=B4,"OK","PAS OK")</f>
+        <v>OK</v>
+      </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="B5">
-        <v>5</v>
-      </c>
-      <c r="C5">
-        <v>5</v>
-      </c>
       <c r="D5" t="str">
-        <f>IF(C5=B5,"OK","PAS OK")</f>
+        <f t="shared" ref="D5:D31" si="0">IF(C5=B5,"OK","PAS OK")</f>
         <v>OK</v>
       </c>
     </row>
@@ -602,7 +656,7 @@
         <v>8</v>
       </c>
       <c r="D6" t="str">
-        <f t="shared" ref="D6:D32" si="0">IF(C6=B6,"OK","PAS OK")</f>
+        <f t="shared" si="0"/>
         <v>OK</v>
       </c>
     </row>
@@ -637,6 +691,12 @@
       <c r="A10" t="s">
         <v>12</v>
       </c>
+      <c r="B10">
+        <v>60</v>
+      </c>
+      <c r="C10">
+        <v>60</v>
+      </c>
       <c r="D10" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -647,10 +707,10 @@
         <v>13</v>
       </c>
       <c r="B11">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C11">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D11" t="str">
         <f t="shared" si="0"/>
@@ -662,10 +722,10 @@
         <v>14</v>
       </c>
       <c r="B12">
-        <v>62</v>
+        <v>93</v>
       </c>
       <c r="C12">
-        <v>62</v>
+        <v>93</v>
       </c>
       <c r="D12" t="str">
         <f t="shared" si="0"/>
@@ -677,14 +737,11 @@
         <v>15</v>
       </c>
       <c r="B13">
-        <v>93</v>
-      </c>
-      <c r="C13">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="D13" t="str">
         <f t="shared" si="0"/>
-        <v>OK</v>
+        <v>PAS OK</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -692,11 +749,14 @@
         <v>16</v>
       </c>
       <c r="B14">
-        <v>96</v>
+        <v>17</v>
+      </c>
+      <c r="C14">
+        <v>17</v>
       </c>
       <c r="D14" t="str">
         <f t="shared" si="0"/>
-        <v>PAS OK</v>
+        <v>OK</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -704,14 +764,14 @@
         <v>17</v>
       </c>
       <c r="B15">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C15">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="D15" t="str">
         <f t="shared" si="0"/>
-        <v>OK</v>
+        <v>PAS OK</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -719,26 +779,20 @@
         <v>18</v>
       </c>
       <c r="B16">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C16">
-        <v>41</v>
+        <v>7</v>
       </c>
       <c r="D16" t="str">
         <f t="shared" si="0"/>
-        <v>PAS OK</v>
+        <v>OK</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>19</v>
       </c>
-      <c r="B17">
-        <v>7</v>
-      </c>
-      <c r="C17">
-        <v>7</v>
-      </c>
       <c r="D17" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -748,24 +802,25 @@
       <c r="A18" t="s">
         <v>20</v>
       </c>
+      <c r="C18" s="3"/>
       <c r="D18" t="str">
-        <f t="shared" si="0"/>
-        <v>OK</v>
+        <f>IF(C18=B19,"OK","PAS OK")</f>
+        <v>PAS OK</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-      <c r="D19" t="str">
-        <f t="shared" si="0"/>
-        <v>PAS OK</v>
+      <c r="B19" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" t="e">
+        <f>IF(C19=#REF!,"OK","PAS OK")</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -773,7 +828,7 @@
         <v>22</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D20" t="str">
         <f t="shared" si="0"/>
@@ -785,7 +840,7 @@
         <v>23</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D21" t="str">
         <f t="shared" si="0"/>
@@ -797,7 +852,7 @@
         <v>24</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D22" t="str">
         <f t="shared" si="0"/>
@@ -809,7 +864,7 @@
         <v>25</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D23" t="str">
         <f t="shared" si="0"/>
@@ -820,7 +875,10 @@
       <c r="A24" t="s">
         <v>26</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24">
+        <v>5</v>
+      </c>
+      <c r="C24" t="s">
         <v>35</v>
       </c>
       <c r="D24" t="str">
@@ -833,10 +891,10 @@
         <v>27</v>
       </c>
       <c r="B25">
-        <v>5</v>
+        <v>99999999</v>
       </c>
       <c r="C25" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D25" t="str">
         <f t="shared" si="0"/>
@@ -848,10 +906,10 @@
         <v>28</v>
       </c>
       <c r="B26">
-        <v>99999999</v>
+        <v>-1</v>
       </c>
       <c r="C26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D26" t="str">
         <f t="shared" si="0"/>
@@ -863,14 +921,14 @@
         <v>29</v>
       </c>
       <c r="B27">
-        <v>-1</v>
-      </c>
-      <c r="C27" t="s">
-        <v>36</v>
+        <v>80</v>
+      </c>
+      <c r="C27">
+        <v>80</v>
       </c>
       <c r="D27" t="str">
         <f t="shared" si="0"/>
-        <v>PAS OK</v>
+        <v>OK</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -878,10 +936,10 @@
         <v>30</v>
       </c>
       <c r="B28">
-        <v>80</v>
+        <v>300</v>
       </c>
       <c r="C28">
-        <v>80</v>
+        <v>300</v>
       </c>
       <c r="D28" t="str">
         <f t="shared" si="0"/>
@@ -893,10 +951,10 @@
         <v>31</v>
       </c>
       <c r="B29">
-        <v>300</v>
+        <v>150</v>
       </c>
       <c r="C29">
-        <v>300</v>
+        <v>150</v>
       </c>
       <c r="D29" t="str">
         <f t="shared" si="0"/>
@@ -908,14 +966,14 @@
         <v>32</v>
       </c>
       <c r="B30">
-        <v>150</v>
+        <v>205</v>
       </c>
       <c r="C30">
-        <v>150</v>
+        <v>250</v>
       </c>
       <c r="D30" t="str">
         <f t="shared" si="0"/>
-        <v>OK</v>
+        <v>PAS OK</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -923,33 +981,21 @@
         <v>33</v>
       </c>
       <c r="B31">
-        <v>205</v>
+        <v>190</v>
       </c>
       <c r="C31">
-        <v>250</v>
+        <v>190</v>
       </c>
       <c r="D31" t="str">
         <f t="shared" si="0"/>
-        <v>PAS OK</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32" t="s">
-        <v>34</v>
-      </c>
-      <c r="B32">
-        <v>190</v>
-      </c>
-      <c r="C32">
-        <v>190</v>
-      </c>
-      <c r="D32" t="str">
-        <f t="shared" si="0"/>
         <v>OK</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D5:D32">
+  <conditionalFormatting sqref="D4:D31">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"ok"</formula>
+    </cfRule>
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -960,9 +1006,6 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
-      <formula>"ok"</formula>
-    </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
suppression du test next_playerÃ_frame et ajout colonne description
</commit_message>
<xml_diff>
--- a/tests/test_cases_recipes.xlsx
+++ b/tests/test_cases_recipes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\canad\Documents\APP4\INFO\bowlingP\bowling_project\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A55B2E2-3710-4FF7-BC24-BAF68B88EC94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDDB78C0-1EA5-4317-84AC-B27C0401ABB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="68">
   <si>
     <t>Test Name</t>
   </si>
@@ -182,6 +182,99 @@
       </rPr>
       <t>)</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Description </t>
+  </si>
+  <si>
+    <t>Ajoute le score d'un joueur pour une frame, en gérant les strikes, les spares ou les scores normaux.</t>
+  </si>
+  <si>
+    <t>Passe au tour suivant du jeu, en mettant potentiellement à jour les informations de la frame et du joueur.</t>
+  </si>
+  <si>
+    <t>Vérifie que le nombre de quilles abattues est valide dans le contexte de la dernière frame.</t>
+  </si>
+  <si>
+    <t>Vérifie que le nombre de quilles abattues est dans la plage valide (0 à 10).</t>
+  </si>
+  <si>
+    <t>Confirme que le nombre de quilles abattues est cohérent avec le lancer précédent.</t>
+  </si>
+  <si>
+    <t>Vérifie si les lancers dans une frame résultent en un spare et met à jour le score de la frame en conséquence.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Vérifie spécifiquement un strike dans la dernière frame et adapte les lancers suivants.</t>
+  </si>
+  <si>
+    <t>Demande puis valide le nombre de quilles abattues.</t>
+  </si>
+  <si>
+    <t>Calcule le score total basé sur la liste des scores de frame.</t>
+  </si>
+  <si>
+    <t>Teste la logique de calcul des scores pour un scénario de jeu de base.</t>
+  </si>
+  <si>
+    <t>Teste la logique de calcul des scores lorsque toutes les frames sont des strikes.</t>
+  </si>
+  <si>
+    <t>Teste la logique de calcul des scores pour un jeu composé entièrement de spares.</t>
+  </si>
+  <si>
+    <t>Teste la logique de calcul des scores pour divers scénarios de dernière frame impliquant des strikes.</t>
+  </si>
+  <si>
+    <t>Teste la logique de calcul des scores pour divers scénarios de dernière frame impliquant des spares.</t>
+  </si>
+  <si>
+    <t>Teste les scénarios de dernière frame qui ne résultent ni en spare ni en strike.</t>
+  </si>
+  <si>
+    <t>Réinitialise ou efface la liste des joueurs.</t>
+  </si>
+  <si>
+    <t>Teste la fonctionnalité pour ajouter un joueur au jeu.</t>
+  </si>
+  <si>
+    <t>Teste le processus de création d'un joueur et sa justesse.</t>
+  </si>
+  <si>
+    <t>Teste la transition vers la frame du joueur suivant.</t>
+  </si>
+  <si>
+    <t>Teste la configuration initiale du jeu et les conditions de démarrage.</t>
+  </si>
+  <si>
+    <t>Valide les choix des joueurs, comme le nombre de quilles abattues.</t>
+  </si>
+  <si>
+    <t>Teste l'acceptation des choix valides des joueurs.</t>
+  </si>
+  <si>
+    <t>Teste le rejet des choix invalides des joueurs.</t>
+  </si>
+  <si>
+    <t>Teste la gestion par le jeu des entrées de cas limites qui peuvent ne pas être typiques ou attendues.</t>
+  </si>
+  <si>
+    <t>Teste comment le jeu gère un nombre incorrect de joueurs.</t>
+  </si>
+  <si>
+    <t>Teste la logique de calcul des scores pour un jeu standard sans strikes ni spares.</t>
+  </si>
+  <si>
+    <t>Teste la logique de calcul des scores pour un jeu parfait où chaque frame est un strike.</t>
+  </si>
+  <si>
+    <t>Teste la logique de calcul des scores pour un jeu avec des spares à chaque frame.</t>
+  </si>
+  <si>
+    <t>Teste un scénario de jeu avec un nombre égal de strikes et de spares.</t>
+  </si>
+  <si>
+    <t>Teste la logique de calcul des scores pour un jeu avec alternance de strikes et de spares.</t>
   </si>
 </sst>
 </file>
@@ -237,7 +330,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -260,11 +353,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -274,6 +380,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -590,409 +699,503 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="47.109375" customWidth="1"/>
-    <col min="2" max="2" width="48.33203125" customWidth="1"/>
-    <col min="3" max="3" width="30.44140625" customWidth="1"/>
+    <col min="2" max="2" width="125.33203125" customWidth="1"/>
+    <col min="3" max="3" width="48.33203125" customWidth="1"/>
+    <col min="4" max="4" width="30.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="B3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4">
-        <v>5</v>
+      <c r="B4" t="s">
+        <v>40</v>
       </c>
       <c r="C4">
         <v>5</v>
       </c>
-      <c r="D4" t="str">
-        <f>IF(C4=B4,"OK","PAS OK")</f>
-        <v>OK</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="D4">
+        <v>5</v>
+      </c>
+      <c r="E4" t="str">
+        <f>IF(D4=C4,"OK","PAS OK")</f>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="D5" t="str">
-        <f t="shared" ref="D5:D31" si="0">IF(C5=B5,"OK","PAS OK")</f>
-        <v>OK</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="B5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" ref="E5:E31" si="0">IF(D5=C5,"OK","PAS OK")</f>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>8</v>
       </c>
-      <c r="D6" t="str">
-        <f t="shared" si="0"/>
-        <v>OK</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="B6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="0"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>9</v>
       </c>
-      <c r="D7" t="str">
-        <f t="shared" si="0"/>
-        <v>OK</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="B7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="0"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>10</v>
       </c>
-      <c r="D8" t="str">
-        <f t="shared" si="0"/>
-        <v>OK</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="B8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="0"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>11</v>
       </c>
-      <c r="D9" t="str">
-        <f t="shared" si="0"/>
-        <v>OK</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="B9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" si="0"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>12</v>
       </c>
-      <c r="B10">
-        <v>60</v>
+      <c r="B10" t="s">
+        <v>46</v>
       </c>
       <c r="C10">
         <v>60</v>
       </c>
-      <c r="D10" t="str">
-        <f t="shared" si="0"/>
-        <v>OK</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="D10">
+        <v>60</v>
+      </c>
+      <c r="E10" t="str">
+        <f t="shared" si="0"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>13</v>
       </c>
-      <c r="B11">
-        <v>62</v>
+      <c r="B11" t="s">
+        <v>47</v>
       </c>
       <c r="C11">
         <v>62</v>
       </c>
-      <c r="D11" t="str">
-        <f t="shared" si="0"/>
-        <v>OK</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="D11">
+        <v>62</v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" si="0"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>14</v>
       </c>
-      <c r="B12">
-        <v>93</v>
+      <c r="B12" t="s">
+        <v>48</v>
       </c>
       <c r="C12">
         <v>93</v>
       </c>
-      <c r="D12" t="str">
-        <f t="shared" si="0"/>
-        <v>OK</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="D12">
+        <v>93</v>
+      </c>
+      <c r="E12" t="str">
+        <f t="shared" si="0"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>15</v>
       </c>
-      <c r="B13">
+      <c r="B13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13">
         <v>96</v>
       </c>
-      <c r="D13" t="str">
+      <c r="E13" t="str">
         <f t="shared" si="0"/>
         <v>PAS OK</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>16</v>
       </c>
-      <c r="B14">
-        <v>17</v>
+      <c r="B14" t="s">
+        <v>50</v>
       </c>
       <c r="C14">
         <v>17</v>
       </c>
-      <c r="D14" t="str">
-        <f t="shared" si="0"/>
-        <v>OK</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="D14">
+        <v>17</v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" si="0"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>17</v>
       </c>
-      <c r="B15">
+      <c r="B15" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15">
         <v>14</v>
       </c>
-      <c r="C15">
+      <c r="D15">
         <v>41</v>
       </c>
-      <c r="D15" t="str">
+      <c r="E15" t="str">
         <f t="shared" si="0"/>
         <v>PAS OK</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>18</v>
       </c>
-      <c r="B16">
-        <v>7</v>
+      <c r="B16" t="s">
+        <v>52</v>
       </c>
       <c r="C16">
         <v>7</v>
       </c>
-      <c r="D16" t="str">
-        <f t="shared" si="0"/>
-        <v>OK</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="D16">
+        <v>7</v>
+      </c>
+      <c r="E16" t="str">
+        <f t="shared" si="0"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>19</v>
       </c>
-      <c r="D17" t="str">
-        <f t="shared" si="0"/>
-        <v>OK</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="B17" t="s">
+        <v>53</v>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" si="0"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="3"/>
-      <c r="D18" t="str">
-        <f>IF(C18=B19,"OK","PAS OK")</f>
+      <c r="B18" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" s="3"/>
+      <c r="E18" t="str">
+        <f>IF(D18=C19,"OK","PAS OK")</f>
         <v>PAS OK</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>36</v>
+      <c r="B19" t="s">
+        <v>55</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D19" t="e">
-        <f>IF(C19=#REF!,"OK","PAS OK")</f>
+      <c r="D19" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E19" t="e">
+        <f>IF(D19=#REF!,"OK","PAS OK")</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D20" t="str">
+      <c r="E20" t="str">
         <f t="shared" si="0"/>
         <v>PAS OK</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" t="s">
+        <v>57</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D21" t="str">
+      <c r="E21" t="str">
         <f t="shared" si="0"/>
         <v>PAS OK</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D22" t="str">
+      <c r="E22" t="str">
         <f t="shared" si="0"/>
         <v>PAS OK</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D23" t="str">
+      <c r="E23" t="str">
         <f t="shared" si="0"/>
         <v>PAS OK</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>26</v>
       </c>
-      <c r="B24">
+      <c r="B24" t="s">
+        <v>60</v>
+      </c>
+      <c r="C24">
         <v>5</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>35</v>
       </c>
-      <c r="D24" t="str">
+      <c r="E24" t="str">
         <f t="shared" si="0"/>
         <v>PAS OK</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>27</v>
       </c>
-      <c r="B25">
+      <c r="B25" t="s">
+        <v>61</v>
+      </c>
+      <c r="C25">
         <v>99999999</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>35</v>
       </c>
-      <c r="D25" t="str">
+      <c r="E25" t="str">
         <f t="shared" si="0"/>
         <v>PAS OK</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
         <v>28</v>
       </c>
-      <c r="B26">
+      <c r="B26" t="s">
+        <v>62</v>
+      </c>
+      <c r="C26">
         <v>-1</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>35</v>
       </c>
-      <c r="D26" t="str">
+      <c r="E26" t="str">
         <f t="shared" si="0"/>
         <v>PAS OK</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
         <v>29</v>
       </c>
-      <c r="B27">
-        <v>80</v>
+      <c r="B27" t="s">
+        <v>63</v>
       </c>
       <c r="C27">
         <v>80</v>
       </c>
-      <c r="D27" t="str">
-        <f t="shared" si="0"/>
-        <v>OK</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
+      <c r="D27">
+        <v>80</v>
+      </c>
+      <c r="E27" t="str">
+        <f t="shared" si="0"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
         <v>30</v>
       </c>
-      <c r="B28">
-        <v>300</v>
+      <c r="B28" t="s">
+        <v>64</v>
       </c>
       <c r="C28">
         <v>300</v>
       </c>
-      <c r="D28" t="str">
-        <f t="shared" si="0"/>
-        <v>OK</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
+      <c r="D28">
+        <v>300</v>
+      </c>
+      <c r="E28" t="str">
+        <f t="shared" si="0"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
         <v>31</v>
       </c>
-      <c r="B29">
-        <v>150</v>
+      <c r="B29" t="s">
+        <v>65</v>
       </c>
       <c r="C29">
         <v>150</v>
       </c>
-      <c r="D29" t="str">
-        <f t="shared" si="0"/>
-        <v>OK</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
+      <c r="D29">
+        <v>150</v>
+      </c>
+      <c r="E29" t="str">
+        <f t="shared" si="0"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
         <v>32</v>
       </c>
-      <c r="B30">
+      <c r="B30" t="s">
+        <v>66</v>
+      </c>
+      <c r="C30">
         <v>205</v>
       </c>
-      <c r="C30">
+      <c r="D30">
         <v>250</v>
       </c>
-      <c r="D30" t="str">
+      <c r="E30" t="str">
         <f t="shared" si="0"/>
         <v>PAS OK</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:5">
       <c r="A31" t="s">
         <v>33</v>
       </c>
-      <c r="B31">
-        <v>190</v>
+      <c r="B31" t="s">
+        <v>67</v>
       </c>
       <c r="C31">
         <v>190</v>
       </c>
-      <c r="D31" t="str">
+      <c r="D31">
+        <v>190</v>
+      </c>
+      <c r="E31" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D4:D31">
+  <conditionalFormatting sqref="E4:E31">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"ok"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Revert "ajout test système"
</commit_message>
<xml_diff>
--- a/tests/test_cases_recipes.xlsx
+++ b/tests/test_cases_recipes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camar\OneDrive\Documents\Polytech année 4\Qualité Logiciel\bowling_project\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\canad\Documents\APP4\INFO\bowlingP\bowling_project\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60821950-59EB-445F-8A00-51CD40C5B60C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A55B2E2-3710-4FF7-BC24-BAF68B88EC94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
   <si>
     <t>Test Name</t>
   </si>
@@ -182,63 +182,6 @@
       </rPr>
       <t>)</t>
     </r>
-  </si>
-  <si>
-    <t>Test système :</t>
-  </si>
-  <si>
-    <t>- Nombre de joueurs décidé au début cohérent avec nombre de joueurs présent dans la partie, on ne peut pas lancer de partie avec 0 joueur</t>
-  </si>
-  <si>
-    <t>- Nombre de quilles décidé au début cohérent avec nombre de quilles présent dans la partie, on ne peut pas lancer de partie avec 0 quilles</t>
-  </si>
-  <si>
-    <t>- Nombre de tours décidé au début cohérent avec nombre de tours présent dans la partie, on ne peut pas lancer de partie avec 0 tours</t>
-  </si>
-  <si>
-    <t>- Impossibilité de remplir le deuxième lancé avant le premier =&gt; affichage d’un message d’erreur</t>
-  </si>
-  <si>
-    <t>- Impossibilité de mettre un nombre de quilles supérieur aux nombres de quilles restantes lors du second lancé</t>
-  </si>
-  <si>
-    <t>- Impossibilité de renseigner un pseudo vide dans la création des joueurs</t>
-  </si>
-  <si>
-    <t>- Impossibilité de renseigner des valeurs vident lors d’un tour.</t>
-  </si>
-  <si>
-    <t>- Le bouton Reset permet de réinitialiser la fenêtre dans le cas où un joueur se serait trompé en ajoutant des valeurs.</t>
-  </si>
-  <si>
-    <t>Dans un tour classique :</t>
-  </si>
-  <si>
-    <t>- Impossible de renseigner le nombre de quilles du second lancé dans le cas ou il y a un strike au premier lancé</t>
-  </si>
-  <si>
-    <t>Dans le dernier tour :</t>
-  </si>
-  <si>
-    <t>- Si à la dernière frame un joueur note un strike, une nouvelle TextBox s'affiche, mais s'il se rend compte qu'il a fait une erreur et change la valeur, la TextBox ajoutée ne disparaît pas pour autant, mais il peut appuyer sur Reset pour réinitialiser la fenêtre, c'est une solution de contournement.</t>
-  </si>
-  <si>
-    <t>- Si un joueur fait un strike au premier lancé, une troisième TextBox s’affiche, car il a droit à un troisième lancé.</t>
-  </si>
-  <si>
-    <t>- Si un joueur fait un spare, une troisième TextBox s’affiche, car il a droit à un troisième lancé.</t>
-  </si>
-  <si>
-    <t>La gestion des scores :</t>
-  </si>
-  <si>
-    <t>- Le score est affiché au cours de la partie et est calculé au tour suivant et non en temps réel.</t>
-  </si>
-  <si>
-    <t>- Le joueur ayant le score le plus élevé est le gagnant et son nom est affiché dans l’écran de fin de partie</t>
-  </si>
-  <si>
-    <t>- S’il y a plusieurs gagnants, leurs noms sont affichés dans l’écran de fin de partie.</t>
   </si>
 </sst>
 </file>
@@ -321,7 +264,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -330,9 +273,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -650,10 +590,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D56"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -1049,101 +989,6 @@
       <c r="D31" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1">
-      <c r="A38" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1">
-      <c r="A39" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1">
-      <c r="A40" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1">
-      <c r="A41" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1">
-      <c r="A42" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1">
-      <c r="A43" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1">
-      <c r="A44" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1">
-      <c r="A45" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1">
-      <c r="A46" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1">
-      <c r="A47" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1">
-      <c r="A48" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1">
-      <c r="A49" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1">
-      <c r="A50" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1">
-      <c r="A51" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1">
-      <c r="A52" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1">
-      <c r="A53" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1">
-      <c r="A54" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1">
-      <c r="A55" s="4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1">
-      <c r="A56" s="4" t="s">
-        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>